<commit_message>
BQC - View icon & IS - Pick Table - Accept lot filter - Fix
</commit_message>
<xml_diff>
--- a/Doc/Bulk_Data_Master.xlsx
+++ b/Doc/Bulk_Data_Master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Workspace\Watchcase Tracker Titan\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Workspace\Watchcase\TTT-Jan2026\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4F7063-CEF7-4D68-815B-CEC0853E35EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F6B4B-7475-4357-9168-288A8065E969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="80">
   <si>
     <t>S.No</t>
   </si>
@@ -732,11 +732,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A133" sqref="A133:A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -795,7 +795,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="9">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>9</v>
@@ -843,7 +843,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="9">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>53</v>
@@ -866,7 +866,7 @@
         <v>48</v>
       </c>
       <c r="F5" s="9">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>9</v>
@@ -889,7 +889,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="9">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>19</v>
@@ -912,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="9">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>53</v>
@@ -935,7 +935,7 @@
         <v>48</v>
       </c>
       <c r="F8" s="9">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>9</v>
@@ -958,7 +958,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="9">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>19</v>
@@ -981,7 +981,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="9">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>53</v>
@@ -1004,7 +1004,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="9">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>9</v>
@@ -1027,7 +1027,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="9">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>19</v>
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="9">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>53</v>
@@ -1073,7 +1073,7 @@
         <v>48</v>
       </c>
       <c r="F14" s="9">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>9</v>
@@ -1096,7 +1096,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="9">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>19</v>
@@ -1119,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="9">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>53</v>
@@ -1142,7 +1142,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="9">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>9</v>
@@ -1165,7 +1165,7 @@
         <v>50</v>
       </c>
       <c r="F18" s="9">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>19</v>
@@ -1188,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="9">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>53</v>
@@ -1211,7 +1211,7 @@
         <v>48</v>
       </c>
       <c r="F20" s="9">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>9</v>
@@ -1234,7 +1234,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="9">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>19</v>
@@ -1257,7 +1257,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="9">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>53</v>
@@ -1280,7 +1280,7 @@
         <v>48</v>
       </c>
       <c r="F23" s="9">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>9</v>
@@ -1303,7 +1303,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="9">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>19</v>
@@ -1326,7 +1326,7 @@
         <v>8</v>
       </c>
       <c r="F25" s="9">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>53</v>
@@ -1349,7 +1349,7 @@
         <v>48</v>
       </c>
       <c r="F26" s="9">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>9</v>
@@ -1372,7 +1372,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="9">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>19</v>
@@ -1395,7 +1395,7 @@
         <v>8</v>
       </c>
       <c r="F28" s="9">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>53</v>
@@ -1418,7 +1418,7 @@
         <v>48</v>
       </c>
       <c r="F29" s="9">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>9</v>
@@ -1441,7 +1441,7 @@
         <v>50</v>
       </c>
       <c r="F30" s="9">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>19</v>
@@ -1464,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="9">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>53</v>
@@ -1487,7 +1487,7 @@
         <v>48</v>
       </c>
       <c r="F32" s="9">
-        <v>70</v>
+        <v>185</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>9</v>
@@ -1510,7 +1510,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="9">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>19</v>
@@ -1533,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="F34" s="9">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>53</v>
@@ -1556,7 +1556,7 @@
         <v>48</v>
       </c>
       <c r="F35" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>9</v>
@@ -1579,7 +1579,7 @@
         <v>50</v>
       </c>
       <c r="F36" s="9">
-        <v>110</v>
+        <v>205</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>19</v>
@@ -1602,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="9">
-        <v>120</v>
+        <v>210</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>53</v>
@@ -1625,7 +1625,7 @@
         <v>48</v>
       </c>
       <c r="F38" s="9">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>9</v>
@@ -1648,7 +1648,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="9">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>19</v>
@@ -1671,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="F40" s="9">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>53</v>
@@ -1694,7 +1694,7 @@
         <v>48</v>
       </c>
       <c r="F41" s="9">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>9</v>
@@ -1717,7 +1717,7 @@
         <v>50</v>
       </c>
       <c r="F42" s="9">
-        <v>40</v>
+        <v>235</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>19</v>
@@ -1740,7 +1740,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="9">
-        <v>50</v>
+        <v>240</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>53</v>
@@ -1763,10 +1763,2126 @@
         <v>48</v>
       </c>
       <c r="F44" s="9">
+        <v>245</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="9">
+        <v>35</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="9">
+        <v>40</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="9">
+        <v>45</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="9">
+        <v>50</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="9">
+        <v>55</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="9">
         <v>60</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>9</v>
+      <c r="G50" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" s="9">
+        <v>65</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="9">
+        <v>70</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="9">
+        <v>75</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="9">
+        <v>80</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="9">
+        <v>85</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="9">
+        <v>90</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="9">
+        <v>95</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" s="9">
+        <v>100</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="9">
+        <v>105</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" s="9">
+        <v>110</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F61" s="9">
+        <v>115</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="9">
+        <v>120</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F63" s="9">
+        <v>125</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F64" s="9">
+        <v>130</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="9">
+        <v>135</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F66" s="9">
+        <v>140</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F67" s="9">
+        <v>145</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="9">
+        <v>150</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" s="9">
+        <v>155</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" s="9">
+        <v>160</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="9">
+        <v>165</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F72" s="9">
+        <v>170</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F73" s="9">
+        <v>175</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="9">
+        <v>180</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="9">
+        <v>185</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F76" s="9">
+        <v>190</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="9">
+        <v>195</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" s="9">
+        <v>200</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" s="9">
+        <v>205</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="9">
+        <v>210</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F81" s="9">
+        <v>215</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F82" s="9">
+        <v>220</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="9">
+        <v>225</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F84" s="9">
+        <v>230</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F85" s="9">
+        <v>235</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="9">
+        <v>240</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F87" s="9">
+        <v>245</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F88" s="9">
+        <v>35</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F89" s="9">
+        <v>40</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" s="9">
+        <v>45</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" s="9">
+        <v>50</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F92" s="9">
+        <v>55</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="9">
+        <v>60</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F94" s="9">
+        <v>65</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F95" s="9">
+        <v>70</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="9">
+        <v>75</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" s="9">
+        <v>80</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F98" s="9">
+        <v>85</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="9">
+        <v>90</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F100" s="9">
+        <v>95</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F101" s="9">
+        <v>100</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="9">
+        <v>105</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="5">
+        <v>102</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F103" s="9">
+        <v>110</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F104" s="9">
+        <v>115</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="5">
+        <v>104</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="9">
+        <v>120</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F106" s="9">
+        <v>125</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="5">
+        <v>106</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F107" s="9">
+        <v>130</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="9">
+        <v>135</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F109" s="9">
+        <v>140</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F110" s="9">
+        <v>145</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="5">
+        <v>110</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="9">
+        <v>150</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="5">
+        <v>111</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F112" s="9">
+        <v>155</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="5">
+        <v>112</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F113" s="9">
+        <v>160</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="5">
+        <v>113</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" s="9">
+        <v>165</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="5">
+        <v>114</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F115" s="9">
+        <v>170</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="5">
+        <v>115</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F116" s="9">
+        <v>175</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="5">
+        <v>116</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="9">
+        <v>180</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="5">
+        <v>117</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F118" s="9">
+        <v>185</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="5">
+        <v>118</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D119" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F119" s="9">
+        <v>190</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="5">
+        <v>119</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F120" s="9">
+        <v>195</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="5">
+        <v>120</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D121" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F121" s="9">
+        <v>200</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="5">
+        <v>121</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D122" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F122" s="9">
+        <v>205</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="5">
+        <v>122</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="9">
+        <v>210</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="5">
+        <v>123</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F124" s="9">
+        <v>215</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="5">
+        <v>124</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D125" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F125" s="9">
+        <v>220</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="5">
+        <v>125</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D126" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="9">
+        <v>225</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="5">
+        <v>126</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C127" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F127" s="9">
+        <v>230</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="5">
+        <v>127</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C128" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D128" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F128" s="9">
+        <v>235</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="5">
+        <v>128</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="9">
+        <v>240</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="5">
+        <v>129</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C130" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F130" s="9">
+        <v>245</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="5">
+        <v>130</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F131" s="9">
+        <v>200</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="5">
+        <v>131</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C132" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D132" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F132" s="9">
+        <v>205</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="5">
+        <v>132</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D133" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="9">
+        <v>210</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="5">
+        <v>133</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="9">
+        <v>150</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="5">
+        <v>134</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F135" s="9">
+        <v>35</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="5">
+        <v>135</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F136" s="9">
+        <v>40</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>